<commit_message>
Added columns where we can record whether papers were used in Traveset 1998 or Verdu&Traveset 2004
</commit_message>
<xml_diff>
--- a/Seed Handling database_foranalysis.xlsx
+++ b/Seed Handling database_foranalysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16000" windowHeight="11540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Available Papers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3115" uniqueCount="1659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3117" uniqueCount="1661">
   <si>
     <t>notes</t>
   </si>
@@ -5146,6 +5146,12 @@
   </si>
   <si>
     <t xml:space="preserve">Anacardium microsepalum, Annona hypoglauca, Astrocaryum jauary, Byrsonima amazonica, Byrsonima sp., Carapa guinensis, Cecropia membranacea, Duguetia marcgraviana, Ficus sp., Genipa americana, Hevea brasiliensis, Hevea spruceana, Licania apetala, Licania sp., Lucuma dissepala, Mabea nitida, Nectandra amazonum, Neolabatia cuprea, Piranhea trifoliolata, Protium sp., Randia armata, Simaba guianensis, Sorocea duckei, Symeria paniculata, Tabebuia barbata, Unonopsis matthewsii, Virola surinamensis, Elaeocarpaceae, Cucurbitaceae, Lecythidaceae </t>
+  </si>
+  <si>
+    <t>Traveset1998</t>
+  </si>
+  <si>
+    <t>Traveset2004</t>
   </si>
 </sst>
 </file>
@@ -5707,9 +5713,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE206"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5776,8 +5782,12 @@
       <c r="P1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="Q1" s="2" t="s">
+        <v>1659</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>1660</v>
+      </c>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>

</xml_diff>